<commit_message>
Correction to cell reference
</commit_message>
<xml_diff>
--- a/example_data/experimental/2024-01-15_SeqLib_SLJS034_NOMADS_BatchBC.xlsx
+++ b/example_data/experimental/2024-01-15_SeqLib_SLJS034_NOMADS_BatchBC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbridges\Desktop\experimental\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\example_data\experimental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F5A263-9D99-4F37-9A99-35FC1876D8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323AE1C4-9A1F-4A51-9E6A-C3B3AE638C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29625" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
     <definedName name="flowcell_status">Assay!$C$69</definedName>
     <definedName name="flowcell_targetmass">Assay!$B$59</definedName>
     <definedName name="flowcell_usage_hrs">Assay!$C$70</definedName>
-    <definedName name="library_washbuffer">Assay!$P$44</definedName>
+    <definedName name="library_washbuffer">Assay!$C$52</definedName>
     <definedName name="missing_qc_resolution">reference!$B$7</definedName>
     <definedName name="seq_platform">Assay!$C$67</definedName>
     <definedName name="vol_calc">reference!$B$6</definedName>
@@ -2979,87 +2979,50 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3074,41 +3037,78 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -4234,7 +4234,7 @@
   </sheetPr>
   <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
@@ -4244,181 +4244,181 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="96" t="s">
         <v>386</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
-      <c r="H1" s="131"/>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="131"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="132" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="98" t="s">
         <v>443</v>
       </c>
-      <c r="D2" s="132"/>
-      <c r="E2" s="132"/>
-      <c r="F2" s="132"/>
-      <c r="G2" s="115" t="s">
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="115"/>
-      <c r="J2" s="133" t="s">
+      <c r="H2" s="99"/>
+      <c r="J2" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="133"/>
+      <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="96"/>
-      <c r="C3" s="134" t="s">
+      <c r="B3" s="97"/>
+      <c r="C3" s="101" t="s">
         <v>436</v>
       </c>
-      <c r="D3" s="134"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="134"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
       <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="135" t="s">
+      <c r="J3" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="135"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="96"/>
-      <c r="C4" s="132" t="s">
+      <c r="B4" s="97"/>
+      <c r="C4" s="98" t="s">
         <v>444</v>
       </c>
-      <c r="D4" s="132"/>
-      <c r="E4" s="132"/>
-      <c r="F4" s="132"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
       <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="136" t="s">
+      <c r="J4" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="136"/>
+      <c r="K4" s="103"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="126"/>
-      <c r="C5" s="111" t="str">
+      <c r="B5" s="104"/>
+      <c r="C5" s="105" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v>SLJS034</v>
       </c>
-      <c r="D5" s="111"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="127" t="s">
+      <c r="J5" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="127"/>
+      <c r="K5" s="106"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="126" t="s">
+      <c r="A6" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="126"/>
-      <c r="C6" s="128" t="str">
+      <c r="B6" s="104"/>
+      <c r="C6" s="107" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v>2024-01-15_SeqLib_SLJS034</v>
       </c>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
       <c r="G6" s="5"/>
-      <c r="J6" s="127"/>
-      <c r="K6" s="127"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129" t="s">
+      <c r="A7" s="108" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="129"/>
-      <c r="C7" s="130" t="s">
+      <c r="B7" s="108"/>
+      <c r="C7" s="109" t="s">
         <v>442</v>
       </c>
-      <c r="D7" s="130"/>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
       <c r="G7" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129" t="s">
+      <c r="A8" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="129"/>
-      <c r="C8" s="130" t="s">
+      <c r="B8" s="108"/>
+      <c r="C8" s="109" t="s">
         <v>445</v>
       </c>
-      <c r="D8" s="130"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="130"/>
+      <c r="D8" s="109"/>
+      <c r="E8" s="109"/>
+      <c r="F8" s="109"/>
       <c r="G8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="122" t="s">
+      <c r="A9" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="122"/>
-      <c r="C9" s="123" t="str">
+      <c r="B9" s="110"/>
+      <c r="C9" s="111" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v>NOMADS_BatchBC</v>
       </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
       <c r="G9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="122"/>
-      <c r="C10" s="123" t="str">
+      <c r="B10" s="110"/>
+      <c r="C10" s="111" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v>2024-01-15_SeqLib_SLJS034_NOMADS_BatchBC</v>
       </c>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="123"/>
-      <c r="H10" s="123"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="111"/>
+      <c r="H10" s="111"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="96" t="s">
+      <c r="A11" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="96"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="27">
         <v>34</v>
       </c>
@@ -4428,34 +4428,34 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="96" t="s">
+      <c r="A12" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="124" t="s">
+      <c r="B12" s="97"/>
+      <c r="C12" s="112" t="s">
         <v>446</v>
       </c>
-      <c r="D12" s="124"/>
-      <c r="E12" s="124"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="124"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
+      <c r="K12" s="112"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="124"/>
-      <c r="D13" s="124"/>
-      <c r="E13" s="124"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
-      <c r="K13" s="124"/>
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
+      <c r="K13" s="112"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="6"/>
@@ -4466,11 +4466,11 @@
       </c>
       <c r="C15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="I15" s="125" t="s">
+      <c r="I15" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="125"/>
-      <c r="K15" s="125"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
@@ -4502,119 +4502,119 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="107" t="s">
+      <c r="A18" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="107"/>
-      <c r="C18" s="107"/>
-      <c r="D18" s="121" t="s">
+      <c r="B18" s="114"/>
+      <c r="C18" s="114"/>
+      <c r="D18" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="121"/>
-      <c r="F18" s="121" t="str">
+      <c r="E18" s="115"/>
+      <c r="F18" s="115" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x34 (µl)</v>
       </c>
-      <c r="G18" s="121"/>
-      <c r="I18" s="101" t="s">
+      <c r="G18" s="115"/>
+      <c r="I18" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="J18" s="101"/>
+      <c r="J18" s="116"/>
       <c r="K18" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="105" t="s">
+      <c r="A19" s="117" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="105"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="116" t="s">
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="118" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="116"/>
-      <c r="F19" s="117" t="s">
+      <c r="E19" s="118"/>
+      <c r="F19" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="117"/>
-      <c r="I19" s="99">
+      <c r="G19" s="119"/>
+      <c r="I19" s="120">
         <v>20</v>
       </c>
-      <c r="J19" s="99"/>
+      <c r="J19" s="120"/>
       <c r="K19" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="105" t="s">
+      <c r="A20" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="105"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="116" t="str">
+      <c r="B20" s="117"/>
+      <c r="C20" s="117"/>
+      <c r="D20" s="118" t="str">
         <f>CONCATENATE(endrepair_maxvol, " - x")</f>
         <v>10 - x</v>
       </c>
-      <c r="E20" s="116"/>
-      <c r="F20" s="117" t="s">
+      <c r="E20" s="118"/>
+      <c r="F20" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="117"/>
-      <c r="I20" s="99">
+      <c r="G20" s="119"/>
+      <c r="I20" s="120">
         <v>65</v>
       </c>
-      <c r="J20" s="99"/>
+      <c r="J20" s="120"/>
       <c r="K20" s="8">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="3" customFormat="1" ht="25.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="105" t="s">
+      <c r="A21" s="117" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="105"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="119">
+      <c r="B21" s="117"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="121">
         <v>1.4</v>
       </c>
-      <c r="E21" s="119"/>
-      <c r="F21" s="117">
+      <c r="E21" s="121"/>
+      <c r="F21" s="119">
         <f>SUM(D21*exp_rxns*(1+$D$17))</f>
         <v>52.36</v>
       </c>
-      <c r="G21" s="117"/>
-      <c r="I21" s="99">
+      <c r="G21" s="119"/>
+      <c r="I21" s="120">
         <v>4</v>
       </c>
-      <c r="J21" s="99"/>
+      <c r="J21" s="120"/>
       <c r="K21" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="105" t="s">
+      <c r="A22" s="117" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="105"/>
-      <c r="C22" s="105"/>
-      <c r="D22" s="119">
+      <c r="B22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="121">
         <v>0.6</v>
       </c>
-      <c r="E22" s="119"/>
-      <c r="F22" s="117">
+      <c r="E22" s="121"/>
+      <c r="F22" s="119">
         <f>SUM(D22*exp_rxns*(1+$D$17))</f>
         <v>22.44</v>
       </c>
-      <c r="G22" s="117"/>
+      <c r="G22" s="119"/>
     </row>
     <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
-      <c r="D23" s="120">
+      <c r="D23" s="122">
         <f>SUM(D21:D22)+endrepair_maxvol</f>
         <v>12</v>
       </c>
-      <c r="E23" s="120"/>
+      <c r="E23" s="122"/>
       <c r="F23" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D21:D22)," µl of MM to each")</f>
         <v>Add 2 µl of MM to each</v>
@@ -4639,103 +4639,103 @@
       </c>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="107"/>
-      <c r="C26" s="107"/>
-      <c r="D26" s="121" t="s">
+      <c r="B26" s="114"/>
+      <c r="C26" s="114"/>
+      <c r="D26" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="121"/>
-      <c r="F26" s="121" t="str">
+      <c r="E26" s="115"/>
+      <c r="F26" s="115" t="str">
         <f>CONCATENATE("MM x",exp_rxns," (µl)")</f>
         <v>MM x34 (µl)</v>
       </c>
-      <c r="G26" s="121"/>
-      <c r="I26" s="101" t="s">
+      <c r="G26" s="115"/>
+      <c r="I26" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="101"/>
+      <c r="J26" s="116"/>
       <c r="K26" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="105" t="s">
+      <c r="A27" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="105"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="116">
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="118">
         <v>0.5</v>
       </c>
-      <c r="E27" s="116"/>
-      <c r="F27" s="117" t="s">
+      <c r="E27" s="118"/>
+      <c r="F27" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="117"/>
-      <c r="I27" s="99">
+      <c r="G27" s="119"/>
+      <c r="I27" s="120">
         <v>20</v>
       </c>
-      <c r="J27" s="99"/>
+      <c r="J27" s="120"/>
       <c r="K27" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="105" t="s">
+      <c r="A28" s="117" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="116">
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="118">
         <v>6</v>
       </c>
-      <c r="E28" s="116"/>
-      <c r="F28" s="117">
+      <c r="E28" s="118"/>
+      <c r="F28" s="119">
         <f>SUM(D28*exp_rxns*(1+$D$25))</f>
         <v>224.4</v>
       </c>
-      <c r="G28" s="117"/>
-      <c r="I28" s="99">
+      <c r="G28" s="119"/>
+      <c r="I28" s="120">
         <v>65</v>
       </c>
-      <c r="J28" s="99"/>
+      <c r="J28" s="120"/>
       <c r="K28" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="105" t="s">
+      <c r="A29" s="117" t="s">
         <v>39</v>
       </c>
-      <c r="B29" s="105"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="116">
+      <c r="B29" s="117"/>
+      <c r="C29" s="117"/>
+      <c r="D29" s="118">
         <v>0.2</v>
       </c>
-      <c r="E29" s="116"/>
-      <c r="F29" s="117">
+      <c r="E29" s="118"/>
+      <c r="F29" s="119">
         <f>SUM(D29*exp_rxns*(1+$D$25))</f>
         <v>7.4800000000000013</v>
       </c>
-      <c r="G29" s="117"/>
-      <c r="I29" s="99">
+      <c r="G29" s="119"/>
+      <c r="I29" s="120">
         <v>8</v>
       </c>
-      <c r="J29" s="99"/>
+      <c r="J29" s="120"/>
       <c r="K29" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="8"/>
-      <c r="D30" s="118">
+      <c r="D30" s="123">
         <f>SUM(D27:D29)+D23</f>
         <v>18.7</v>
       </c>
-      <c r="E30" s="118"/>
+      <c r="E30" s="123"/>
       <c r="F30" s="13" t="str">
         <f>CONCATENATE("Add ",SUM(D28:D29)," µl of MM to each")</f>
         <v>Add 6.2 µl of MM to each</v>
@@ -4807,19 +4807,19 @@
       <c r="G35" s="26"/>
     </row>
     <row r="36" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="114" t="s">
+      <c r="A36" s="128" t="s">
         <v>422</v>
       </c>
-      <c r="B36" s="115"/>
-      <c r="C36" s="115"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="115"/>
-      <c r="F36" s="115"/>
-      <c r="G36" s="115"/>
-      <c r="H36" s="115"/>
-      <c r="I36" s="115"/>
-      <c r="J36" s="115"/>
-      <c r="K36" s="115"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="99"/>
+      <c r="G36" s="99"/>
+      <c r="H36" s="99"/>
+      <c r="I36" s="99"/>
+      <c r="J36" s="99"/>
+      <c r="K36" s="99"/>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="71" t="s">
@@ -4842,10 +4842,10 @@
       <c r="C38" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D38" s="103" t="s">
+      <c r="D38" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="103"/>
+      <c r="E38" s="124"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="17">
@@ -4858,11 +4858,11 @@
       <c r="C39" s="34">
         <v>1</v>
       </c>
-      <c r="D39" s="113">
+      <c r="D39" s="125">
         <f>SUM(B39*C39)</f>
         <v>86</v>
       </c>
-      <c r="E39" s="113"/>
+      <c r="E39" s="125"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -4888,97 +4888,97 @@
       </c>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="101" t="s">
+      <c r="A43" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="B43" s="101"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="102" t="s">
+      <c r="B43" s="116"/>
+      <c r="C43" s="116"/>
+      <c r="D43" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="E43" s="102"/>
-      <c r="I43" s="101" t="s">
+      <c r="E43" s="126"/>
+      <c r="I43" s="116" t="s">
         <v>27</v>
       </c>
-      <c r="J43" s="101"/>
+      <c r="J43" s="116"/>
       <c r="K43" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="105" t="s">
+      <c r="A44" s="117" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="105"/>
-      <c r="C44" s="105"/>
-      <c r="D44" s="104">
+      <c r="B44" s="117"/>
+      <c r="C44" s="117"/>
+      <c r="D44" s="127">
         <f>IF(B39="",adaptlig_dna_maxvol,IF(SUM(adaptlig_targetmass/D39)&gt;adaptlig_dna_maxvol,adaptlig_dna_maxvol,SUM(adaptlig_targetmass/D39)))</f>
         <v>17.441860465116278</v>
       </c>
-      <c r="E44" s="104"/>
+      <c r="E44" s="127"/>
       <c r="F44" s="5"/>
-      <c r="I44" s="99" t="s">
+      <c r="I44" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="99"/>
+      <c r="J44" s="120"/>
       <c r="K44" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="105" t="s">
+      <c r="A45" s="117" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="105"/>
-      <c r="C45" s="105"/>
-      <c r="D45" s="104">
+      <c r="B45" s="117"/>
+      <c r="C45" s="117"/>
+      <c r="D45" s="127">
         <f>IFERROR(SUM(adaptlig_dna_maxvol-D44),"")</f>
         <v>12.558139534883722</v>
       </c>
-      <c r="E45" s="104"/>
+      <c r="E45" s="127"/>
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="105" t="s">
+      <c r="A46" s="117" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="105"/>
-      <c r="C46" s="105"/>
-      <c r="D46" s="111">
+      <c r="B46" s="117"/>
+      <c r="C46" s="117"/>
+      <c r="D46" s="105">
         <v>5</v>
       </c>
-      <c r="E46" s="111"/>
+      <c r="E46" s="105"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="105" t="s">
+      <c r="A47" s="117" t="s">
         <v>381</v>
       </c>
-      <c r="B47" s="105"/>
-      <c r="C47" s="105"/>
-      <c r="D47" s="111">
+      <c r="B47" s="117"/>
+      <c r="C47" s="117"/>
+      <c r="D47" s="105">
         <f>SUM(adaptlig_rxn_vol/5)</f>
         <v>10</v>
       </c>
-      <c r="E47" s="111"/>
+      <c r="E47" s="105"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="105" t="s">
+      <c r="A48" s="117" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="105"/>
-      <c r="C48" s="105"/>
-      <c r="D48" s="111">
+      <c r="B48" s="117"/>
+      <c r="C48" s="117"/>
+      <c r="D48" s="105">
         <f>SUM(adaptlig_rxn_vol/10)</f>
         <v>5</v>
       </c>
-      <c r="E48" s="111"/>
+      <c r="E48" s="105"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D49" s="112">
+      <c r="D49" s="129">
         <f>SUM(D44:D48)</f>
         <v>50</v>
       </c>
-      <c r="E49" s="112"/>
+      <c r="E49" s="129"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
@@ -4997,20 +4997,20 @@
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" s="110" t="s">
+      <c r="A53" s="132" t="s">
         <v>384</v>
       </c>
-      <c r="B53" s="110"/>
-      <c r="C53" s="110"/>
-      <c r="D53" s="110"/>
-      <c r="E53" s="110"/>
-      <c r="F53" s="110"/>
-      <c r="G53" s="110"/>
-      <c r="H53" s="110"/>
-      <c r="I53" s="110"/>
-      <c r="J53" s="110"/>
-      <c r="K53" s="110"/>
-      <c r="L53" s="110"/>
+      <c r="B53" s="132"/>
+      <c r="C53" s="132"/>
+      <c r="D53" s="132"/>
+      <c r="E53" s="132"/>
+      <c r="F53" s="132"/>
+      <c r="G53" s="132"/>
+      <c r="H53" s="132"/>
+      <c r="I53" s="132"/>
+      <c r="J53" s="132"/>
+      <c r="K53" s="132"/>
+      <c r="L53" s="132"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="71" t="s">
@@ -5028,42 +5028,42 @@
       <c r="L54" s="88"/>
     </row>
     <row r="55" spans="1:12" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="107" t="s">
+      <c r="A55" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="B55" s="107"/>
-      <c r="C55" s="107" t="s">
+      <c r="B55" s="114"/>
+      <c r="C55" s="114" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="107"/>
-      <c r="E55" s="107" t="s">
+      <c r="D55" s="114"/>
+      <c r="E55" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="F55" s="107"/>
-      <c r="G55" s="107" t="s">
+      <c r="F55" s="114"/>
+      <c r="G55" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="H55" s="107"/>
+      <c r="H55" s="114"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A56" s="108">
+      <c r="A56" s="130">
         <f>SUM(adaptlig_rxn_vol*0.5)</f>
         <v>25</v>
       </c>
-      <c r="B56" s="108"/>
-      <c r="C56" s="109">
+      <c r="B56" s="130"/>
+      <c r="C56" s="131">
         <v>75</v>
       </c>
-      <c r="D56" s="109"/>
-      <c r="E56" s="109">
+      <c r="D56" s="131"/>
+      <c r="E56" s="131">
         <v>1</v>
       </c>
-      <c r="F56" s="109"/>
-      <c r="G56" s="99">
+      <c r="F56" s="131"/>
+      <c r="G56" s="120">
         <f>SUM(C56*E56)</f>
         <v>75</v>
       </c>
-      <c r="H56" s="99"/>
+      <c r="H56" s="120"/>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
@@ -5084,61 +5084,61 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="101" t="s">
+      <c r="A60" s="116" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="101"/>
-      <c r="C60" s="101"/>
-      <c r="D60" s="102" t="s">
+      <c r="B60" s="116"/>
+      <c r="C60" s="116"/>
+      <c r="D60" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="E60" s="102"/>
+      <c r="E60" s="126"/>
     </row>
     <row r="61" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="103" t="s">
+      <c r="A61" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="103"/>
-      <c r="C61" s="103"/>
-      <c r="D61" s="104">
+      <c r="B61" s="124"/>
+      <c r="C61" s="124"/>
+      <c r="D61" s="127">
         <f>IF(C56="",flowcell_maxvol,IF(SUM(flowcell_targetmass/G56)&gt;flowcell_maxvol,flowcell_maxvol,SUM(flowcell_targetmass/G56)))</f>
         <v>10.666666666666666</v>
       </c>
-      <c r="E61" s="104"/>
+      <c r="E61" s="127"/>
     </row>
     <row r="62" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="103" t="s">
+      <c r="A62" s="124" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="103"/>
-      <c r="C62" s="103"/>
-      <c r="D62" s="104">
+      <c r="B62" s="124"/>
+      <c r="C62" s="124"/>
+      <c r="D62" s="127">
         <f>IFERROR((IF(SUM(12-D61)=0,"-",SUM(12-D61))),"")</f>
         <v>1.3333333333333339</v>
       </c>
-      <c r="E62" s="104"/>
+      <c r="E62" s="127"/>
     </row>
     <row r="63" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="105" t="s">
+      <c r="A63" s="117" t="s">
         <v>387</v>
       </c>
-      <c r="B63" s="105"/>
-      <c r="C63" s="105"/>
-      <c r="D63" s="106">
+      <c r="B63" s="117"/>
+      <c r="C63" s="117"/>
+      <c r="D63" s="133">
         <v>37.5</v>
       </c>
-      <c r="E63" s="106"/>
+      <c r="E63" s="133"/>
     </row>
     <row r="64" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="105" t="s">
+      <c r="A64" s="117" t="s">
         <v>388</v>
       </c>
-      <c r="B64" s="105"/>
-      <c r="C64" s="105"/>
-      <c r="D64" s="106">
+      <c r="B64" s="117"/>
+      <c r="C64" s="117"/>
+      <c r="D64" s="133">
         <v>25.5</v>
       </c>
-      <c r="E64" s="106"/>
+      <c r="E64" s="133"/>
       <c r="F64" s="5" t="s">
         <v>55</v>
       </c>
@@ -5150,194 +5150,92 @@
       <c r="C66" s="5"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="96" t="s">
+      <c r="A67" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="96"/>
-      <c r="C67" s="98" t="s">
+      <c r="B67" s="97"/>
+      <c r="C67" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="D67" s="98"/>
+      <c r="D67" s="135"/>
       <c r="E67" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="96" t="s">
+      <c r="A68" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="B68" s="96"/>
-      <c r="C68" s="99" t="s">
+      <c r="B68" s="97"/>
+      <c r="C68" s="120" t="s">
         <v>448</v>
       </c>
-      <c r="D68" s="99"/>
+      <c r="D68" s="120"/>
     </row>
     <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="96" t="s">
+      <c r="A69" s="97" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="96"/>
-      <c r="C69" s="97" t="s">
+      <c r="B69" s="97"/>
+      <c r="C69" s="134" t="s">
         <v>294</v>
       </c>
-      <c r="D69" s="97"/>
+      <c r="D69" s="134"/>
     </row>
     <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="96" t="s">
+      <c r="A70" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="B70" s="96"/>
-      <c r="C70" s="100">
-        <v>10</v>
-      </c>
-      <c r="D70" s="100"/>
+      <c r="B70" s="97"/>
+      <c r="C70" s="136">
+        <v>10</v>
+      </c>
+      <c r="D70" s="136"/>
       <c r="E70" s="9" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="96" t="s">
+      <c r="A71" s="97" t="s">
         <v>63</v>
       </c>
-      <c r="B71" s="96"/>
-      <c r="C71" s="98" t="s">
+      <c r="B71" s="97"/>
+      <c r="C71" s="135" t="s">
         <v>64</v>
       </c>
-      <c r="D71" s="98"/>
+      <c r="D71" s="135"/>
       <c r="E71" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="96" t="s">
+      <c r="A72" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="B72" s="96"/>
-      <c r="C72" s="97">
+      <c r="B72" s="97"/>
+      <c r="C72" s="134">
         <v>476</v>
       </c>
-      <c r="D72" s="97"/>
+      <c r="D72" s="134"/>
       <c r="E72" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="96" t="s">
+      <c r="A73" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="B73" s="96"/>
-      <c r="C73" s="97">
-        <v>10</v>
-      </c>
-      <c r="D73" s="97"/>
+      <c r="B73" s="97"/>
+      <c r="C73" s="134">
+        <v>10</v>
+      </c>
+      <c r="D73" s="134"/>
       <c r="E73" s="9" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="116">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="I43:J43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="A48:C48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="A53:L53"/>
-    <mergeCell ref="A60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="A61:C61"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:E64"/>
     <mergeCell ref="A72:B72"/>
     <mergeCell ref="C72:D72"/>
     <mergeCell ref="A73:B73"/>
@@ -5352,6 +5250,108 @@
     <mergeCell ref="C70:D70"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="C71:D71"/>
+    <mergeCell ref="A60:C60"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="A61:C61"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="A63:C63"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="I43:J43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
   </mergeCells>
   <conditionalFormatting sqref="B59">
     <cfRule type="expression" dxfId="15" priority="8">
@@ -17085,7 +17085,7 @@
       </c>
       <c r="N2" t="str">
         <f>IF(LEN(library_washbuffer)&gt;0,library_washbuffer,"")</f>
-        <v/>
+        <v>LFB</v>
       </c>
       <c r="O2">
         <f>IF(DNAconc_library=0,"",DNAconc_library)</f>

</xml_diff>